<commit_message>
Sprememba v preglednici 2
</commit_message>
<xml_diff>
--- a/preglednica.xlsx
+++ b/preglednica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TestGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F796D80-8D9D-4125-A398-BF394B2E4ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D404B4F-C859-45CB-B0B9-54F8AA832E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +505,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>